<commit_message>
v1.1 chart update and 5 s alarm
</commit_message>
<xml_diff>
--- a/Python/Chart.xlsx
+++ b/Python/Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jahe0003\Documents\GitHub\group4\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4C05F46-C3C5-41D3-89AF-B3CB7B62A3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DD8E1E-CAC3-409E-A754-F54A4FEE2C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{56323C84-709E-4261-9D5E-79FB32C8AA74}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <t>GP0</t>
   </si>
@@ -152,12 +152,6 @@
     <t>Gyro VIN</t>
   </si>
   <si>
-    <t>H-bridge 2A</t>
-  </si>
-  <si>
-    <t>H-bridge 1A</t>
-  </si>
-  <si>
     <t>Ultra Ground</t>
   </si>
   <si>
@@ -174,6 +168,93 @@
   </si>
   <si>
     <t>Buzzer -</t>
+  </si>
+  <si>
+    <t>L293D EN 1</t>
+  </si>
+  <si>
+    <t>L293D EN2</t>
+  </si>
+  <si>
+    <t>L293D IN 1</t>
+  </si>
+  <si>
+    <t>L293D IN 2</t>
+  </si>
+  <si>
+    <t>L293D IN 3</t>
+  </si>
+  <si>
+    <t>L293D IN 4</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico pins</t>
+  </si>
+  <si>
+    <t>L293D Pins</t>
+  </si>
+  <si>
+    <t>EN1</t>
+  </si>
+  <si>
+    <t>IN1</t>
+  </si>
+  <si>
+    <t>OUT1</t>
+  </si>
+  <si>
+    <t>GRD</t>
+  </si>
+  <si>
+    <t>OUT2</t>
+  </si>
+  <si>
+    <t>IN2</t>
+  </si>
+  <si>
+    <t>Vin(motor)</t>
+  </si>
+  <si>
+    <t>Vin(L293D)</t>
+  </si>
+  <si>
+    <t>IN4</t>
+  </si>
+  <si>
+    <t>OUT4</t>
+  </si>
+  <si>
+    <t>OUT3</t>
+  </si>
+  <si>
+    <t>IN3</t>
+  </si>
+  <si>
+    <t>EN2</t>
+  </si>
+  <si>
+    <t>ExtraPowerPack+</t>
+  </si>
+  <si>
+    <t>ExtraPowerPack-</t>
+  </si>
+  <si>
+    <t>BatteryPack+</t>
+  </si>
+  <si>
+    <t>BatteryPack-</t>
+  </si>
+  <si>
+    <t>Motor1 F+</t>
+  </si>
+  <si>
+    <t>Motor1 B-</t>
+  </si>
+  <si>
+    <t>Motor2 F+</t>
+  </si>
+  <si>
+    <t>Motor2 B-</t>
   </si>
 </sst>
 </file>
@@ -226,10 +307,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,375 +626,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBA3ADA-71D1-4E70-AF96-DE1050C9A84F}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="H17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32">
+      <c r="B41" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="D41" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41">
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>32</v>
       </c>
     </row>
@@ -927,6 +1129,69 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Is_Collaboration_Space_Locked xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Student_Groups xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Self_Registration_Enabled xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Templates xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Invited_Teachers xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Invited_Students xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <CultureName xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <AppVersion xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <LMS_Mappings xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <FolderType xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Teachers xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Distribution_Groups xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <_activity xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Owner xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Self_Registration_Enabled0 xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Math_Settings xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <TeamsChannelId xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <NotebookType xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
+    <Students xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009DF117138A37404FB83FC3B2C5BC5D29" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74db7562f9ef2055fdb61bfe87eb4441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2f4b350a-1af6-4fee-b681-c1850f550807" xmlns:ns4="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14dbfb8aeb21dee41450f70622754f02" ns3:_="" ns4:_="">
     <xsd:import namespace="2f4b350a-1af6-4fee-b681-c1850f550807"/>
@@ -1381,70 +1646,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CB273E-52A2-4A9C-AC5B-750DFDBB6A83}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="2f4b350a-1af6-4fee-b681-c1850f550807"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Is_Collaboration_Space_Locked xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Student_Groups xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Self_Registration_Enabled xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Templates xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Invited_Teachers xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Invited_Students xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <CultureName xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <AppVersion xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <LMS_Mappings xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <FolderType xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Teachers xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Distribution_Groups xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <_activity xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Owner xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Self_Registration_Enabled0 xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Math_Settings xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <TeamsChannelId xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <NotebookType xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc" xsi:nil="true"/>
-    <Students xmlns="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F89249-B44E-4AB0-BC1D-22EC4FDBE203}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{693CB477-A7F9-40E9-9A30-96E6D7A70B3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1461,29 +1688,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F89249-B44E-4AB0-BC1D-22EC4FDBE203}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CB273E-52A2-4A9C-AC5B-750DFDBB6A83}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2f4b350a-1af6-4fee-b681-c1850f550807"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="80a390f3-b1f1-4c66-86e8-cdc1c820ecfc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>